<commit_message>
add worksheet regex support
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -5,11 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="report_2025" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="report_2024" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="5">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -315,11 +317,11 @@
       </c>
       <c r="C2" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0853171828051312</v>
+        <v>0.159426480568704</v>
       </c>
       <c r="D2" s="1" t="n">
         <f aca="false">B2*C2</f>
-        <v>0.102380619366157</v>
+        <v>0.191311776682445</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -331,11 +333,11 @@
       </c>
       <c r="C3" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.162944632827307</v>
+        <v>0.51364823414182</v>
       </c>
       <c r="D3" s="1" t="n">
         <f aca="false">B3*C3</f>
-        <v>0.22812248595823</v>
+        <v>0.719107527798548</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -347,11 +349,11 @@
       </c>
       <c r="C4" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.523586871063524</v>
+        <v>0.455489237701594</v>
       </c>
       <c r="D4" s="1" t="n">
         <f aca="false">B4*C4</f>
-        <v>0.837738993701639</v>
+        <v>0.728782780322551</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -363,11 +365,11 @@
       </c>
       <c r="C5" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.373941332912911</v>
+        <v>0.171155246434188</v>
       </c>
       <c r="D5" s="1" t="n">
         <f aca="false">B5*C5</f>
-        <v>0.673094399243239</v>
+        <v>0.308079443581538</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -379,11 +381,11 @@
       </c>
       <c r="C6" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.846698453860823</v>
+        <v>0.679769054193288</v>
       </c>
       <c r="D6" s="1" t="n">
         <f aca="false">B6*C6</f>
-        <v>1.69339690772165</v>
+        <v>1.35953810838658</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -395,11 +397,11 @@
       </c>
       <c r="C7" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.478354205436458</v>
+        <v>0.822591705812616</v>
       </c>
       <c r="D7" s="1" t="n">
         <f aca="false">B7*C7</f>
-        <v>1.05237925196021</v>
+        <v>1.80970175278776</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -411,11 +413,11 @@
       </c>
       <c r="C8" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.457824681272092</v>
+        <v>0.693282028359595</v>
       </c>
       <c r="D8" s="1" t="n">
         <f aca="false">B8*C8</f>
-        <v>1.09877923505302</v>
+        <v>1.66387686806303</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -427,11 +429,11 @@
       </c>
       <c r="C9" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.259326781893959</v>
+        <v>0.234640086658423</v>
       </c>
       <c r="D9" s="1" t="n">
         <f aca="false">B9*C9</f>
-        <v>0.674249632924295</v>
+        <v>0.6100642253119</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -443,11 +445,11 @@
       </c>
       <c r="C10" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.191115792985224</v>
+        <v>0.671040671208846</v>
       </c>
       <c r="D10" s="1" t="n">
         <f aca="false">B10*C10</f>
-        <v>0.535124220358628</v>
+        <v>1.87891387938477</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -459,11 +461,11 @@
       </c>
       <c r="C11" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.110172034227686</v>
+        <v>0.903004960512994</v>
       </c>
       <c r="D11" s="1" t="n">
         <f aca="false">B11*C11</f>
-        <v>0.330516102683057</v>
+        <v>2.70901488153898</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -475,11 +477,11 @@
       </c>
       <c r="C12" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.575955312896135</v>
+        <v>0.371607814882663</v>
       </c>
       <c r="D12" s="1" t="n">
         <f aca="false">B12*C12</f>
-        <v>1.84305700126763</v>
+        <v>1.18914500762452</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -491,11 +493,11 @@
       </c>
       <c r="C13" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.948740234044863</v>
+        <v>0.570552319864988</v>
       </c>
       <c r="D13" s="1" t="n">
         <f aca="false">B13*C13</f>
-        <v>3.22571679575254</v>
+        <v>1.93987788754096</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -507,11 +509,11 @@
       </c>
       <c r="C14" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.309292793454416</v>
+        <v>0.408819319593148</v>
       </c>
       <c r="D14" s="1" t="n">
         <f aca="false">B14*C14</f>
-        <v>1.1134540564359</v>
+        <v>1.47174955053533</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -523,11 +525,11 @@
       </c>
       <c r="C15" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.738754873655623</v>
+        <v>0.760103559385365</v>
       </c>
       <c r="D15" s="1" t="n">
         <f aca="false">B15*C15</f>
-        <v>2.80726851989137</v>
+        <v>2.88839352566439</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -539,11 +541,11 @@
       </c>
       <c r="C16" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.256045020234222</v>
+        <v>0.806775988074501</v>
       </c>
       <c r="D16" s="1" t="n">
         <f aca="false">B16*C16</f>
-        <v>1.02418008093689</v>
+        <v>3.227103952298</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -555,11 +557,11 @@
       </c>
       <c r="C17" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.581097679705695</v>
+        <v>0.419939053551517</v>
       </c>
       <c r="D17" s="1" t="n">
         <f aca="false">B17*C17</f>
-        <v>2.44061025476392</v>
+        <v>1.76374402491637</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -571,11 +573,11 @@
       </c>
       <c r="C18" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.395444330101124</v>
+        <v>0.151616090794187</v>
       </c>
       <c r="D18" s="1" t="n">
         <f aca="false">B18*C18</f>
-        <v>1.73995505244495</v>
+        <v>0.667110799494421</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -587,11 +589,11 @@
       </c>
       <c r="C19" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0222658956881396</v>
+        <v>0.489215438576684</v>
       </c>
       <c r="D19" s="1" t="n">
         <f aca="false">B19*C19</f>
-        <v>0.102423120165442</v>
+        <v>2.25039101745275</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -603,11 +605,11 @@
       </c>
       <c r="C20" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.270950398049495</v>
+        <v>0.365803181827466</v>
       </c>
       <c r="D20" s="1" t="n">
         <f aca="false">B20*C20</f>
-        <v>1.30056191063758</v>
+        <v>1.75585527277184</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -655,11 +657,11 @@
       </c>
       <c r="C27" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.893043847732413</v>
+        <v>0.985455269883803</v>
       </c>
       <c r="D27" s="1" t="n">
         <f aca="false">B27*C27</f>
-        <v>5.53687185594096</v>
+        <v>6.10982267327958</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -671,11 +673,11 @@
       </c>
       <c r="C28" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.186927908511883</v>
+        <v>0.488731627573232</v>
       </c>
       <c r="D28" s="1" t="n">
         <f aca="false">B28*C28</f>
-        <v>1.19633861447605</v>
+        <v>3.12788241646869</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -687,11 +689,11 @@
       </c>
       <c r="C29" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.821025909503494</v>
+        <v>0.446665468065157</v>
       </c>
       <c r="D29" s="1" t="n">
         <f aca="false">B29*C29</f>
-        <v>5.41877100272306</v>
+        <v>2.94799208923004</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -703,11 +705,11 @@
       </c>
       <c r="C30" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.41073782430262</v>
+        <v>0.687828384667626</v>
       </c>
       <c r="D30" s="1" t="n">
         <f aca="false">B30*C30</f>
-        <v>2.79301720525782</v>
+        <v>4.67723301573985</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -719,11 +721,11 @@
       </c>
       <c r="C31" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.46111164545401</v>
+        <v>0.0228403116554626</v>
       </c>
       <c r="D31" s="1" t="n">
         <f aca="false">B31*C31</f>
-        <v>3.22778151817807</v>
+        <v>0.159882181588238</v>
       </c>
     </row>
   </sheetData>
@@ -742,9 +744,925 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:D31"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H33" activeCellId="0" sqref="H33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="n">
+        <v>45901</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.508579079725685</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <f aca="false">B2*C2</f>
+        <v>0.610294895670822</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
+        <v>45902</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.423575995782322</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <f aca="false">B3*C3</f>
+        <v>0.593006394095251</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.570514361346204</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <f aca="false">B4*C4</f>
+        <v>0.912822978153926</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
+        <v>45904</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.384401839643234</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <f aca="false">B5*C5</f>
+        <v>0.691923311357821</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="n">
+        <v>45905</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.697028308986843</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <f aca="false">B6*C6</f>
+        <v>1.39405661797369</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="n">
+        <v>45906</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.842566369353412</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <f aca="false">B7*C7</f>
+        <v>1.85364601257751</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="n">
+        <v>45907</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.240167149378899</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <f aca="false">B8*C8</f>
+        <v>0.576401158509357</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="n">
+        <v>45908</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.250621868726903</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <f aca="false">B9*C9</f>
+        <v>0.651616858689949</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="n">
+        <v>45909</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.505557742506714</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <f aca="false">B10*C10</f>
+        <v>1.4155616790188</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="n">
+        <v>45910</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.827431258789879</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <f aca="false">B11*C11</f>
+        <v>2.48229377636964</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="n">
+        <v>45911</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.265280297632011</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <f aca="false">B12*C12</f>
+        <v>0.848896952422435</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="n">
+        <v>45912</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.818920424936508</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <f aca="false">B13*C13</f>
+        <v>2.78432944478413</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="n">
+        <v>45913</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.853323279254522</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <f aca="false">B14*C14</f>
+        <v>3.07196380531628</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="n">
+        <v>45914</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.572422846194997</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <f aca="false">B15*C15</f>
+        <v>2.17520681554099</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="n">
+        <v>45915</v>
+      </c>
+      <c r="B16" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.347644273743432</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <f aca="false">B16*C16</f>
+        <v>1.39057709497373</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="n">
+        <v>45916</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.650755574996196</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <f aca="false">B17*C17</f>
+        <v>2.73317341498402</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="n">
+        <v>45917</v>
+      </c>
+      <c r="B18" s="1" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.354760546468549</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <f aca="false">B18*C18</f>
+        <v>1.56094640446161</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="n">
+        <v>45918</v>
+      </c>
+      <c r="B19" s="1" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.528775025997077</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <f aca="false">B19*C19</f>
+        <v>2.43236511958655</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="n">
+        <v>45919</v>
+      </c>
+      <c r="B20" s="1" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.0166792257822102</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <f aca="false">B20*C20</f>
+        <v>0.0800602837546091</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="n">
+        <v>45926</v>
+      </c>
+      <c r="B27" s="1" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.93443526356643</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <f aca="false">B27*C27</f>
+        <v>5.79349863411187</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="n">
+        <v>45927</v>
+      </c>
+      <c r="B28" s="1" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.877163376543674</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <f aca="false">B28*C28</f>
+        <v>5.61384560987951</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="n">
+        <v>45928</v>
+      </c>
+      <c r="B29" s="1" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.879686076358565</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <f aca="false">B29*C29</f>
+        <v>5.80592810396653</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2" t="n">
+        <v>45929</v>
+      </c>
+      <c r="B30" s="1" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.839198363145994</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <f aca="false">B30*C30</f>
+        <v>5.70654886939276</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="n">
+        <v>45930</v>
+      </c>
+      <c r="B31" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.0755128133813096</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <f aca="false">B31*C31</f>
+        <v>0.528589693669167</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D31"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H33" activeCellId="0" sqref="H33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="n">
+        <v>45901</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.562530205378862</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <f aca="false">B2*C2</f>
+        <v>0.675036246454634</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
+        <v>45902</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.716378698529286</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <f aca="false">B3*C3</f>
+        <v>1.002930177941</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.32356078847016</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <f aca="false">B4*C4</f>
+        <v>0.517697261552256</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
+        <v>45904</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.380751257799798</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <f aca="false">B5*C5</f>
+        <v>0.685352264039636</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="n">
+        <v>45905</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.156010540441412</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <f aca="false">B6*C6</f>
+        <v>0.312021080882823</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="n">
+        <v>45906</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.490028482048216</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <f aca="false">B7*C7</f>
+        <v>1.07806266050608</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="n">
+        <v>45907</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.339518823890797</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <f aca="false">B8*C8</f>
+        <v>0.814845177337913</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="n">
+        <v>45908</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.487747311954685</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <f aca="false">B9*C9</f>
+        <v>1.26814301108218</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="n">
+        <v>45909</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.347918120133841</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <f aca="false">B10*C10</f>
+        <v>0.974170736374756</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="n">
+        <v>45910</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.2255909413269</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <f aca="false">B11*C11</f>
+        <v>0.6767728239807</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="n">
+        <v>45911</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.660288887972121</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <f aca="false">B12*C12</f>
+        <v>2.11292444151079</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="n">
+        <v>45912</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.22197713055995</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <f aca="false">B13*C13</f>
+        <v>0.754722243903829</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="n">
+        <v>45913</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.301933192865377</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <f aca="false">B14*C14</f>
+        <v>1.08695949431536</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="n">
+        <v>45914</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.0468912795720362</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <f aca="false">B15*C15</f>
+        <v>0.178186862373738</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="n">
+        <v>45915</v>
+      </c>
+      <c r="B16" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.623347263891054</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <f aca="false">B16*C16</f>
+        <v>2.49338905556422</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="n">
+        <v>45916</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.0886238947883603</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <f aca="false">B17*C17</f>
+        <v>0.372220358111113</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="n">
+        <v>45917</v>
+      </c>
+      <c r="B18" s="1" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.467364827386421</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <f aca="false">B18*C18</f>
+        <v>2.05640524050025</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="n">
+        <v>45918</v>
+      </c>
+      <c r="B19" s="1" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.60263001758906</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <f aca="false">B19*C19</f>
+        <v>2.77209808090968</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="n">
+        <v>45919</v>
+      </c>
+      <c r="B20" s="1" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.479880123660462</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <f aca="false">B20*C20</f>
+        <v>2.30342459357022</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="n">
+        <v>45926</v>
+      </c>
+      <c r="B27" s="1" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.284438945918143</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <f aca="false">B27*C27</f>
+        <v>1.76352146469249</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="n">
+        <v>45927</v>
+      </c>
+      <c r="B28" s="1" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.0652978471996168</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <f aca="false">B28*C28</f>
+        <v>0.417906222077547</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="n">
+        <v>45928</v>
+      </c>
+      <c r="B29" s="1" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.614351614258322</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <f aca="false">B29*C29</f>
+        <v>4.05472065410492</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2" t="n">
+        <v>45929</v>
+      </c>
+      <c r="B30" s="1" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.902601112006274</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <f aca="false">B30*C30</f>
+        <v>6.13768756164267</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="n">
+        <v>45930</v>
+      </c>
+      <c r="B31" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.310056468115094</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <f aca="false">B31*C31</f>
+        <v>2.17039527680566</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="B2:E35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -778,11 +1696,11 @@
       </c>
       <c r="D6" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.104468991052867</v>
+        <v>0.562820218499161</v>
       </c>
       <c r="E6" s="4" t="n">
         <f aca="false">C6*D6</f>
-        <v>0.12536278926344</v>
+        <v>0.675384262198993</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -794,11 +1712,11 @@
       </c>
       <c r="D7" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.919199423026761</v>
+        <v>0.782557439297352</v>
       </c>
       <c r="E7" s="4" t="n">
         <f aca="false">C7*D7</f>
-        <v>1.28687919223747</v>
+        <v>1.09558041501629</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -810,11 +1728,11 @@
       </c>
       <c r="D8" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.918130082215861</v>
+        <v>0.0935883001147127</v>
       </c>
       <c r="E8" s="4" t="n">
         <f aca="false">C8*D8</f>
-        <v>1.46900813154538</v>
+        <v>0.14974128018354</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -826,11 +1744,11 @@
       </c>
       <c r="D9" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.999077629182963</v>
+        <v>0.364416315505873</v>
       </c>
       <c r="E9" s="4" t="n">
         <f aca="false">C9*D9</f>
-        <v>1.79833973252933</v>
+        <v>0.655949367910572</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -842,11 +1760,11 @@
       </c>
       <c r="D10" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.133132869230573</v>
+        <v>0.759499053723507</v>
       </c>
       <c r="E10" s="4" t="n">
         <f aca="false">C10*D10</f>
-        <v>0.266265738461145</v>
+        <v>1.51899810744701</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -858,11 +1776,11 @@
       </c>
       <c r="D11" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.649135962420038</v>
+        <v>0.108946058363007</v>
       </c>
       <c r="E11" s="4" t="n">
         <f aca="false">C11*D11</f>
-        <v>1.42809911732408</v>
+        <v>0.239681328398616</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -874,11 +1792,11 @@
       </c>
       <c r="D12" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0563295393132169</v>
+        <v>0.379112338213373</v>
       </c>
       <c r="E12" s="4" t="n">
         <f aca="false">C12*D12</f>
-        <v>0.13519089435172</v>
+        <v>0.909869611712095</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -896,11 +1814,11 @@
       </c>
       <c r="D14" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.167867549096577</v>
+        <v>0.788240508100484</v>
       </c>
       <c r="E14" s="4" t="n">
         <f aca="false">C14*D14</f>
-        <v>0.470029137470415</v>
+        <v>2.20707342268136</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -912,11 +1830,11 @@
       </c>
       <c r="D15" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.335937312582318</v>
+        <v>0.388704088257291</v>
       </c>
       <c r="E15" s="4" t="n">
         <f aca="false">C15*D15</f>
-        <v>1.00781193774696</v>
+        <v>1.16611226477187</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -928,11 +1846,11 @@
       </c>
       <c r="D16" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.128369827498604</v>
+        <v>0.250711678563211</v>
       </c>
       <c r="E16" s="4" t="n">
         <f aca="false">C16*D16</f>
-        <v>0.410783447995531</v>
+        <v>0.802277371402275</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -944,11 +1862,11 @@
       </c>
       <c r="D17" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.961360349355039</v>
+        <v>0.970293613271688</v>
       </c>
       <c r="E17" s="4" t="n">
         <f aca="false">C17*D17</f>
-        <v>3.26862518780713</v>
+        <v>3.29899828512374</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -960,11 +1878,11 @@
       </c>
       <c r="D18" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.218462592877777</v>
+        <v>0.109833332851171</v>
       </c>
       <c r="E18" s="4" t="n">
         <f aca="false">C18*D18</f>
-        <v>0.786465334359998</v>
+        <v>0.395399998264216</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -976,11 +1894,11 @@
       </c>
       <c r="D19" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.980705655199514</v>
+        <v>0.887470553904978</v>
       </c>
       <c r="E19" s="4" t="n">
         <f aca="false">C19*D19</f>
-        <v>3.72668148975815</v>
+        <v>3.37238810483892</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -992,11 +1910,11 @@
       </c>
       <c r="D20" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.421109485078522</v>
+        <v>0.540961276882063</v>
       </c>
       <c r="E20" s="4" t="n">
         <f aca="false">C20*D20</f>
-        <v>1.68443794031409</v>
+        <v>2.16384510752825</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1008,11 +1926,11 @@
       </c>
       <c r="D21" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0856897764460628</v>
+        <v>0.407942444953334</v>
       </c>
       <c r="E21" s="4" t="n">
         <f aca="false">C21*D21</f>
-        <v>0.359897061073464</v>
+        <v>1.713358268804</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1024,11 +1942,11 @@
       </c>
       <c r="D22" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.581871234137503</v>
+        <v>0.0107587276576826</v>
       </c>
       <c r="E22" s="4" t="n">
         <f aca="false">C22*D22</f>
-        <v>2.56023343020502</v>
+        <v>0.0473384016938033</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1040,11 +1958,11 @@
       </c>
       <c r="D23" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.867917617497504</v>
+        <v>0.785105241442041</v>
       </c>
       <c r="E23" s="4" t="n">
         <f aca="false">C23*D23</f>
-        <v>3.99242104048852</v>
+        <v>3.61148411063339</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1056,11 +1974,11 @@
       </c>
       <c r="D24" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.303233103726268</v>
+        <v>0.854772440090416</v>
       </c>
       <c r="E24" s="4" t="n">
         <f aca="false">C24*D24</f>
-        <v>1.45551889788609</v>
+        <v>4.10290771243399</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1072,11 +1990,11 @@
       </c>
       <c r="D25" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.334493747761719</v>
+        <v>0.738541513372186</v>
       </c>
       <c r="E25" s="4" t="n">
         <f aca="false">C25*D25</f>
-        <v>1.67246873880859</v>
+        <v>3.69270756686093</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1088,11 +2006,11 @@
       </c>
       <c r="D26" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.710165537168018</v>
+        <v>0.630761936458276</v>
       </c>
       <c r="E26" s="4" t="n">
         <f aca="false">C26*D26</f>
-        <v>3.6928607932737</v>
+        <v>3.27996206958303</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1104,11 +2022,11 @@
       </c>
       <c r="D27" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.425046143428015</v>
+        <v>0.292868501995439</v>
       </c>
       <c r="E27" s="4" t="n">
         <f aca="false">C27*D27</f>
-        <v>2.29524917451128</v>
+        <v>1.58148991077537</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1120,11 +2038,11 @@
       </c>
       <c r="D28" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.631416178638113</v>
+        <v>0.653816452420128</v>
       </c>
       <c r="E28" s="4" t="n">
         <f aca="false">C28*D28</f>
-        <v>3.53593060037343</v>
+        <v>3.66137213355272</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1136,11 +2054,11 @@
       </c>
       <c r="D29" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.988324865477955</v>
+        <v>0.635161162264538</v>
       </c>
       <c r="E29" s="4" t="n">
         <f aca="false">C29*D29</f>
-        <v>5.73228421977214</v>
+        <v>3.68393474113432</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1152,11 +2070,11 @@
       </c>
       <c r="D30" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0896346588692452</v>
+        <v>0.305064555747129</v>
       </c>
       <c r="E30" s="4" t="n">
         <f aca="false">C30*D30</f>
-        <v>0.537807953215471</v>
+        <v>1.83038733448277</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1168,11 +2086,11 @@
       </c>
       <c r="D31" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.325916818479995</v>
+        <v>0.137773030809458</v>
       </c>
       <c r="E31" s="4" t="n">
         <f aca="false">C31*D31</f>
-        <v>2.02068427457597</v>
+        <v>0.854192791018641</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1184,11 +2102,11 @@
       </c>
       <c r="D32" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.605182973245689</v>
+        <v>0.352307823427738</v>
       </c>
       <c r="E32" s="4" t="n">
         <f aca="false">C32*D32</f>
-        <v>3.87317102877241</v>
+        <v>2.25477006993753</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1200,11 +2118,11 @@
       </c>
       <c r="D33" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.335851141489944</v>
+        <v>0.986890237361725</v>
       </c>
       <c r="E33" s="4" t="n">
         <f aca="false">C33*D33</f>
-        <v>2.21661753383363</v>
+        <v>6.51347556658738</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1216,11 +2134,11 @@
       </c>
       <c r="D34" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.876350352024899</v>
+        <v>0.037213003376413</v>
       </c>
       <c r="E34" s="4" t="n">
         <f aca="false">C34*D34</f>
-        <v>5.95918239376931</v>
+        <v>0.253048422959608</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1232,11 +2150,11 @@
       </c>
       <c r="D35" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.488708329465445</v>
+        <v>0.692428149632797</v>
       </c>
       <c r="E35" s="4" t="n">
         <f aca="false">C35*D35</f>
-        <v>3.42095830625812</v>
+        <v>4.84699704742958</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix regex matching, review skip rows/cols logic
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="11">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -35,6 +35,25 @@
   </si>
   <si>
     <t xml:space="preserve">total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comments! &amp;
+And notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d</t>
   </si>
   <si>
     <t xml:space="preserve">A beautiful excel dataset</t>
@@ -137,13 +156,17 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -286,15 +309,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H33" activeCellId="0" sqref="H33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -307,9 +330,12 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
+      <c r="A2" s="3" t="n">
         <v>45901</v>
       </c>
       <c r="B2" s="1" t="n">
@@ -317,15 +343,18 @@
       </c>
       <c r="C2" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.159426480568704</v>
+        <v>0.592980327181324</v>
       </c>
       <c r="D2" s="1" t="n">
         <f aca="false">B2*C2</f>
-        <v>0.191311776682445</v>
+        <v>0.711576392617589</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
+      <c r="A3" s="3" t="n">
         <v>45902</v>
       </c>
       <c r="B3" s="1" t="n">
@@ -333,15 +362,18 @@
       </c>
       <c r="C3" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.51364823414182</v>
+        <v>0.461156331167441</v>
       </c>
       <c r="D3" s="1" t="n">
         <f aca="false">B3*C3</f>
-        <v>0.719107527798548</v>
+        <v>0.645618863634417</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
+      <c r="A4" s="3" t="n">
         <v>45903</v>
       </c>
       <c r="B4" s="1" t="n">
@@ -349,15 +381,18 @@
       </c>
       <c r="C4" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.455489237701594</v>
+        <v>0.755480730872139</v>
       </c>
       <c r="D4" s="1" t="n">
         <f aca="false">B4*C4</f>
-        <v>0.728782780322551</v>
+        <v>1.20876916939542</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="n">
+      <c r="A5" s="3" t="n">
         <v>45904</v>
       </c>
       <c r="B5" s="1" t="n">
@@ -365,15 +400,18 @@
       </c>
       <c r="C5" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.171155246434188</v>
+        <v>0.328168498975646</v>
       </c>
       <c r="D5" s="1" t="n">
         <f aca="false">B5*C5</f>
-        <v>0.308079443581538</v>
+        <v>0.590703298156163</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="n">
+      <c r="A6" s="3" t="n">
         <v>45905</v>
       </c>
       <c r="B6" s="1" t="n">
@@ -381,15 +419,18 @@
       </c>
       <c r="C6" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.679769054193288</v>
+        <v>0.0223803928676676</v>
       </c>
       <c r="D6" s="1" t="n">
         <f aca="false">B6*C6</f>
-        <v>1.35953810838658</v>
+        <v>0.0447607857353351</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="n">
+      <c r="A7" s="3" t="n">
         <v>45906</v>
       </c>
       <c r="B7" s="1" t="n">
@@ -397,15 +438,18 @@
       </c>
       <c r="C7" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.822591705812616</v>
+        <v>0.929119092949924</v>
       </c>
       <c r="D7" s="1" t="n">
         <f aca="false">B7*C7</f>
-        <v>1.80970175278776</v>
+        <v>2.04406200448983</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="n">
+      <c r="A8" s="3" t="n">
         <v>45907</v>
       </c>
       <c r="B8" s="1" t="n">
@@ -413,15 +457,18 @@
       </c>
       <c r="C8" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.693282028359595</v>
+        <v>0.568601744224071</v>
       </c>
       <c r="D8" s="1" t="n">
         <f aca="false">B8*C8</f>
-        <v>1.66387686806303</v>
+        <v>1.36464418613777</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="n">
+      <c r="A9" s="3" t="n">
         <v>45908</v>
       </c>
       <c r="B9" s="1" t="n">
@@ -429,15 +476,18 @@
       </c>
       <c r="C9" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.234640086658423</v>
+        <v>0.968928091638573</v>
       </c>
       <c r="D9" s="1" t="n">
         <f aca="false">B9*C9</f>
-        <v>0.6100642253119</v>
+        <v>2.51921303826029</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="n">
+      <c r="A10" s="3" t="n">
         <v>45909</v>
       </c>
       <c r="B10" s="1" t="n">
@@ -445,15 +495,18 @@
       </c>
       <c r="C10" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.671040671208846</v>
+        <v>0.289246590687076</v>
       </c>
       <c r="D10" s="1" t="n">
         <f aca="false">B10*C10</f>
-        <v>1.87891387938477</v>
+        <v>0.809890453923813</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="n">
+      <c r="A11" s="3" t="n">
         <v>45910</v>
       </c>
       <c r="B11" s="1" t="n">
@@ -461,15 +514,18 @@
       </c>
       <c r="C11" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.903004960512994</v>
+        <v>0.461856078551844</v>
       </c>
       <c r="D11" s="1" t="n">
         <f aca="false">B11*C11</f>
-        <v>2.70901488153898</v>
+        <v>1.38556823565553</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="n">
+      <c r="A12" s="3" t="n">
         <v>45911</v>
       </c>
       <c r="B12" s="1" t="n">
@@ -477,15 +533,18 @@
       </c>
       <c r="C12" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.371607814882663</v>
+        <v>0.872045947311451</v>
       </c>
       <c r="D12" s="1" t="n">
         <f aca="false">B12*C12</f>
-        <v>1.18914500762452</v>
+        <v>2.79054703139664</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="n">
+      <c r="A13" s="3" t="n">
         <v>45912</v>
       </c>
       <c r="B13" s="1" t="n">
@@ -493,15 +552,18 @@
       </c>
       <c r="C13" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.570552319864988</v>
+        <v>0.557911833013507</v>
       </c>
       <c r="D13" s="1" t="n">
         <f aca="false">B13*C13</f>
-        <v>1.93987788754096</v>
+        <v>1.89690023224592</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="n">
+      <c r="A14" s="3" t="n">
         <v>45913</v>
       </c>
       <c r="B14" s="1" t="n">
@@ -509,15 +571,18 @@
       </c>
       <c r="C14" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.408819319593148</v>
+        <v>0.592259299650727</v>
       </c>
       <c r="D14" s="1" t="n">
         <f aca="false">B14*C14</f>
-        <v>1.47174955053533</v>
+        <v>2.13213347874262</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="n">
+      <c r="A15" s="3" t="n">
         <v>45914</v>
       </c>
       <c r="B15" s="1" t="n">
@@ -525,15 +590,18 @@
       </c>
       <c r="C15" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.760103559385365</v>
+        <v>0.749204470443236</v>
       </c>
       <c r="D15" s="1" t="n">
         <f aca="false">B15*C15</f>
-        <v>2.88839352566439</v>
+        <v>2.8469769876843</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="n">
+      <c r="A16" s="3" t="n">
         <v>45915</v>
       </c>
       <c r="B16" s="1" t="n">
@@ -541,15 +609,18 @@
       </c>
       <c r="C16" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.806775988074501</v>
+        <v>0.41214992013206</v>
       </c>
       <c r="D16" s="1" t="n">
         <f aca="false">B16*C16</f>
-        <v>3.227103952298</v>
+        <v>1.64859968052824</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="n">
+      <c r="A17" s="3" t="n">
         <v>45916</v>
       </c>
       <c r="B17" s="1" t="n">
@@ -557,15 +628,18 @@
       </c>
       <c r="C17" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.419939053551517</v>
+        <v>0.115977810364039</v>
       </c>
       <c r="D17" s="1" t="n">
         <f aca="false">B17*C17</f>
-        <v>1.76374402491637</v>
+        <v>0.487106803528965</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="n">
+      <c r="A18" s="3" t="n">
         <v>45917</v>
       </c>
       <c r="B18" s="1" t="n">
@@ -573,15 +647,18 @@
       </c>
       <c r="C18" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.151616090794187</v>
+        <v>0.38928931671385</v>
       </c>
       <c r="D18" s="1" t="n">
         <f aca="false">B18*C18</f>
-        <v>0.667110799494421</v>
+        <v>1.71287299354094</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="n">
+      <c r="A19" s="3" t="n">
         <v>45918</v>
       </c>
       <c r="B19" s="1" t="n">
@@ -589,15 +666,18 @@
       </c>
       <c r="C19" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.489215438576684</v>
+        <v>0.0624555707074757</v>
       </c>
       <c r="D19" s="1" t="n">
         <f aca="false">B19*C19</f>
-        <v>2.25039101745275</v>
+        <v>0.287295625254388</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="n">
+      <c r="A20" s="3" t="n">
         <v>45919</v>
       </c>
       <c r="B20" s="1" t="n">
@@ -605,51 +685,54 @@
       </c>
       <c r="C20" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.365803181827466</v>
+        <v>0.509146829772724</v>
       </c>
       <c r="D20" s="1" t="n">
         <f aca="false">B20*C20</f>
-        <v>1.75585527277184</v>
+        <v>2.44390478290907</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2"/>
+      <c r="A21" s="3"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2"/>
+      <c r="A22" s="3"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2"/>
+      <c r="A23" s="3"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2"/>
+      <c r="A24" s="3"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2"/>
+      <c r="A25" s="3"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2"/>
+      <c r="A26" s="3"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="n">
+      <c r="A27" s="3" t="n">
         <v>45926</v>
       </c>
       <c r="B27" s="1" t="n">
@@ -657,15 +740,18 @@
       </c>
       <c r="C27" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.985455269883803</v>
+        <v>0.616528569465793</v>
       </c>
       <c r="D27" s="1" t="n">
         <f aca="false">B27*C27</f>
-        <v>6.10982267327958</v>
+        <v>3.82247713068792</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="n">
+      <c r="A28" s="3" t="n">
         <v>45927</v>
       </c>
       <c r="B28" s="1" t="n">
@@ -673,15 +759,18 @@
       </c>
       <c r="C28" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.488731627573232</v>
+        <v>0.589269358270281</v>
       </c>
       <c r="D28" s="1" t="n">
         <f aca="false">B28*C28</f>
-        <v>3.12788241646869</v>
+        <v>3.7713238929298</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2" t="n">
+      <c r="A29" s="3" t="n">
         <v>45928</v>
       </c>
       <c r="B29" s="1" t="n">
@@ -689,15 +778,18 @@
       </c>
       <c r="C29" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.446665468065157</v>
+        <v>0.95196012242494</v>
       </c>
       <c r="D29" s="1" t="n">
         <f aca="false">B29*C29</f>
-        <v>2.94799208923004</v>
+        <v>6.2829368080046</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="n">
+      <c r="A30" s="3" t="n">
         <v>45929</v>
       </c>
       <c r="B30" s="1" t="n">
@@ -705,15 +797,18 @@
       </c>
       <c r="C30" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.687828384667626</v>
+        <v>0.152080818979886</v>
       </c>
       <c r="D30" s="1" t="n">
         <f aca="false">B30*C30</f>
-        <v>4.67723301573985</v>
+        <v>1.03414956906323</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="n">
+      <c r="A31" s="3" t="n">
         <v>45930</v>
       </c>
       <c r="B31" s="1" t="n">
@@ -721,11 +816,14 @@
       </c>
       <c r="C31" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0228403116554626</v>
+        <v>0.727378756268333</v>
       </c>
       <c r="D31" s="1" t="n">
         <f aca="false">B31*C31</f>
-        <v>0.159882181588238</v>
+        <v>5.09165129387833</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -767,7 +865,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
+      <c r="A2" s="3" t="n">
         <v>45901</v>
       </c>
       <c r="B2" s="1" t="n">
@@ -775,15 +873,15 @@
       </c>
       <c r="C2" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.508579079725685</v>
+        <v>0.409915725504691</v>
       </c>
       <c r="D2" s="1" t="n">
         <f aca="false">B2*C2</f>
-        <v>0.610294895670822</v>
+        <v>0.491898870605629</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
+      <c r="A3" s="3" t="n">
         <v>45902</v>
       </c>
       <c r="B3" s="1" t="n">
@@ -791,15 +889,15 @@
       </c>
       <c r="C3" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.423575995782322</v>
+        <v>0.479215567714237</v>
       </c>
       <c r="D3" s="1" t="n">
         <f aca="false">B3*C3</f>
-        <v>0.593006394095251</v>
+        <v>0.670901794799932</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
+      <c r="A4" s="3" t="n">
         <v>45903</v>
       </c>
       <c r="B4" s="1" t="n">
@@ -807,15 +905,15 @@
       </c>
       <c r="C4" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.570514361346204</v>
+        <v>0.987219905766249</v>
       </c>
       <c r="D4" s="1" t="n">
         <f aca="false">B4*C4</f>
-        <v>0.912822978153926</v>
+        <v>1.579551849226</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="n">
+      <c r="A5" s="3" t="n">
         <v>45904</v>
       </c>
       <c r="B5" s="1" t="n">
@@ -823,15 +921,15 @@
       </c>
       <c r="C5" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.384401839643234</v>
+        <v>0.718140443200571</v>
       </c>
       <c r="D5" s="1" t="n">
         <f aca="false">B5*C5</f>
-        <v>0.691923311357821</v>
+        <v>1.29265279776103</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="n">
+      <c r="A6" s="3" t="n">
         <v>45905</v>
       </c>
       <c r="B6" s="1" t="n">
@@ -839,15 +937,15 @@
       </c>
       <c r="C6" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.697028308986843</v>
+        <v>0.220690416906822</v>
       </c>
       <c r="D6" s="1" t="n">
         <f aca="false">B6*C6</f>
-        <v>1.39405661797369</v>
+        <v>0.441380833813643</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="n">
+      <c r="A7" s="3" t="n">
         <v>45906</v>
       </c>
       <c r="B7" s="1" t="n">
@@ -855,15 +953,15 @@
       </c>
       <c r="C7" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.842566369353412</v>
+        <v>0.310228058455046</v>
       </c>
       <c r="D7" s="1" t="n">
         <f aca="false">B7*C7</f>
-        <v>1.85364601257751</v>
+        <v>0.682501728601101</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="n">
+      <c r="A8" s="3" t="n">
         <v>45907</v>
       </c>
       <c r="B8" s="1" t="n">
@@ -871,15 +969,15 @@
       </c>
       <c r="C8" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.240167149378899</v>
+        <v>0.144901004400117</v>
       </c>
       <c r="D8" s="1" t="n">
         <f aca="false">B8*C8</f>
-        <v>0.576401158509357</v>
+        <v>0.34776241056028</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="n">
+      <c r="A9" s="3" t="n">
         <v>45908</v>
       </c>
       <c r="B9" s="1" t="n">
@@ -887,15 +985,15 @@
       </c>
       <c r="C9" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.250621868726903</v>
+        <v>0.858053694249661</v>
       </c>
       <c r="D9" s="1" t="n">
         <f aca="false">B9*C9</f>
-        <v>0.651616858689949</v>
+        <v>2.23093960504912</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="n">
+      <c r="A10" s="3" t="n">
         <v>45909</v>
       </c>
       <c r="B10" s="1" t="n">
@@ -903,15 +1001,15 @@
       </c>
       <c r="C10" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.505557742506714</v>
+        <v>0.375092982828274</v>
       </c>
       <c r="D10" s="1" t="n">
         <f aca="false">B10*C10</f>
-        <v>1.4155616790188</v>
+        <v>1.05026035191917</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="n">
+      <c r="A11" s="3" t="n">
         <v>45910</v>
       </c>
       <c r="B11" s="1" t="n">
@@ -919,15 +1017,15 @@
       </c>
       <c r="C11" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.827431258789879</v>
+        <v>0.964295185239815</v>
       </c>
       <c r="D11" s="1" t="n">
         <f aca="false">B11*C11</f>
-        <v>2.48229377636964</v>
+        <v>2.89288555571945</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="n">
+      <c r="A12" s="3" t="n">
         <v>45911</v>
       </c>
       <c r="B12" s="1" t="n">
@@ -935,15 +1033,15 @@
       </c>
       <c r="C12" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.265280297632011</v>
+        <v>0.548505216721068</v>
       </c>
       <c r="D12" s="1" t="n">
         <f aca="false">B12*C12</f>
-        <v>0.848896952422435</v>
+        <v>1.75521669350742</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="n">
+      <c r="A13" s="3" t="n">
         <v>45912</v>
       </c>
       <c r="B13" s="1" t="n">
@@ -951,15 +1049,15 @@
       </c>
       <c r="C13" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.818920424936508</v>
+        <v>0.770406082238393</v>
       </c>
       <c r="D13" s="1" t="n">
         <f aca="false">B13*C13</f>
-        <v>2.78432944478413</v>
+        <v>2.61938067961054</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="n">
+      <c r="A14" s="3" t="n">
         <v>45913</v>
       </c>
       <c r="B14" s="1" t="n">
@@ -967,15 +1065,15 @@
       </c>
       <c r="C14" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.853323279254522</v>
+        <v>0.464961098454965</v>
       </c>
       <c r="D14" s="1" t="n">
         <f aca="false">B14*C14</f>
-        <v>3.07196380531628</v>
+        <v>1.67385995443788</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="n">
+      <c r="A15" s="3" t="n">
         <v>45914</v>
       </c>
       <c r="B15" s="1" t="n">
@@ -983,15 +1081,15 @@
       </c>
       <c r="C15" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.572422846194997</v>
+        <v>0.853362062892977</v>
       </c>
       <c r="D15" s="1" t="n">
         <f aca="false">B15*C15</f>
-        <v>2.17520681554099</v>
+        <v>3.24277583899331</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="n">
+      <c r="A16" s="3" t="n">
         <v>45915</v>
       </c>
       <c r="B16" s="1" t="n">
@@ -999,15 +1097,15 @@
       </c>
       <c r="C16" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.347644273743432</v>
+        <v>0.754930555001226</v>
       </c>
       <c r="D16" s="1" t="n">
         <f aca="false">B16*C16</f>
-        <v>1.39057709497373</v>
+        <v>3.0197222200049</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="n">
+      <c r="A17" s="3" t="n">
         <v>45916</v>
       </c>
       <c r="B17" s="1" t="n">
@@ -1015,15 +1113,15 @@
       </c>
       <c r="C17" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.650755574996196</v>
+        <v>0.799090800022823</v>
       </c>
       <c r="D17" s="1" t="n">
         <f aca="false">B17*C17</f>
-        <v>2.73317341498402</v>
+        <v>3.35618136009586</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="n">
+      <c r="A18" s="3" t="n">
         <v>45917</v>
       </c>
       <c r="B18" s="1" t="n">
@@ -1031,15 +1129,15 @@
       </c>
       <c r="C18" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.354760546468549</v>
+        <v>0.873613256221466</v>
       </c>
       <c r="D18" s="1" t="n">
         <f aca="false">B18*C18</f>
-        <v>1.56094640446161</v>
+        <v>3.84389832737445</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="n">
+      <c r="A19" s="3" t="n">
         <v>45918</v>
       </c>
       <c r="B19" s="1" t="n">
@@ -1047,15 +1145,15 @@
       </c>
       <c r="C19" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.528775025997077</v>
+        <v>0.679065430558101</v>
       </c>
       <c r="D19" s="1" t="n">
         <f aca="false">B19*C19</f>
-        <v>2.43236511958655</v>
+        <v>3.12370098056726</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="n">
+      <c r="A20" s="3" t="n">
         <v>45919</v>
       </c>
       <c r="B20" s="1" t="n">
@@ -1063,51 +1161,51 @@
       </c>
       <c r="C20" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0166792257822102</v>
+        <v>0.0770517952113255</v>
       </c>
       <c r="D20" s="1" t="n">
         <f aca="false">B20*C20</f>
-        <v>0.0800602837546091</v>
+        <v>0.369848617014362</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2"/>
+      <c r="A21" s="3"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2"/>
+      <c r="A22" s="3"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2"/>
+      <c r="A23" s="3"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2"/>
+      <c r="A24" s="3"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2"/>
+      <c r="A25" s="3"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2"/>
+      <c r="A26" s="3"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="n">
+      <c r="A27" s="3" t="n">
         <v>45926</v>
       </c>
       <c r="B27" s="1" t="n">
@@ -1115,15 +1213,15 @@
       </c>
       <c r="C27" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.93443526356643</v>
+        <v>0.562353115009035</v>
       </c>
       <c r="D27" s="1" t="n">
         <f aca="false">B27*C27</f>
-        <v>5.79349863411187</v>
+        <v>3.48658931305602</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="n">
+      <c r="A28" s="3" t="n">
         <v>45927</v>
       </c>
       <c r="B28" s="1" t="n">
@@ -1131,15 +1229,15 @@
       </c>
       <c r="C28" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.877163376543674</v>
+        <v>0.158512599412878</v>
       </c>
       <c r="D28" s="1" t="n">
         <f aca="false">B28*C28</f>
-        <v>5.61384560987951</v>
+        <v>1.01448063624242</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2" t="n">
+      <c r="A29" s="3" t="n">
         <v>45928</v>
       </c>
       <c r="B29" s="1" t="n">
@@ -1147,15 +1245,15 @@
       </c>
       <c r="C29" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.879686076358565</v>
+        <v>0.157170125425718</v>
       </c>
       <c r="D29" s="1" t="n">
         <f aca="false">B29*C29</f>
-        <v>5.80592810396653</v>
+        <v>1.03732282780974</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="n">
+      <c r="A30" s="3" t="n">
         <v>45929</v>
       </c>
       <c r="B30" s="1" t="n">
@@ -1163,15 +1261,15 @@
       </c>
       <c r="C30" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.839198363145994</v>
+        <v>0.280878786265986</v>
       </c>
       <c r="D30" s="1" t="n">
         <f aca="false">B30*C30</f>
-        <v>5.70654886939276</v>
+        <v>1.9099757466087</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="n">
+      <c r="A31" s="3" t="n">
         <v>45930</v>
       </c>
       <c r="B31" s="1" t="n">
@@ -1179,11 +1277,11 @@
       </c>
       <c r="C31" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0755128133813096</v>
+        <v>0.73655538250052</v>
       </c>
       <c r="D31" s="1" t="n">
         <f aca="false">B31*C31</f>
-        <v>0.528589693669167</v>
+        <v>5.15588767750364</v>
       </c>
     </row>
   </sheetData>
@@ -1204,7 +1302,7 @@
   </sheetPr>
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H33" activeCellId="0" sqref="H33"/>
     </sheetView>
   </sheetViews>
@@ -1225,7 +1323,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
+      <c r="A2" s="3" t="n">
         <v>45901</v>
       </c>
       <c r="B2" s="1" t="n">
@@ -1233,15 +1331,15 @@
       </c>
       <c r="C2" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.562530205378862</v>
+        <v>0.0374024587603272</v>
       </c>
       <c r="D2" s="1" t="n">
         <f aca="false">B2*C2</f>
-        <v>0.675036246454634</v>
+        <v>0.0448829505123927</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
+      <c r="A3" s="3" t="n">
         <v>45902</v>
       </c>
       <c r="B3" s="1" t="n">
@@ -1249,15 +1347,15 @@
       </c>
       <c r="C3" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.716378698529286</v>
+        <v>0.31799321295151</v>
       </c>
       <c r="D3" s="1" t="n">
         <f aca="false">B3*C3</f>
-        <v>1.002930177941</v>
+        <v>0.445190498132114</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
+      <c r="A4" s="3" t="n">
         <v>45903</v>
       </c>
       <c r="B4" s="1" t="n">
@@ -1265,15 +1363,15 @@
       </c>
       <c r="C4" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.32356078847016</v>
+        <v>0.579142496003938</v>
       </c>
       <c r="D4" s="1" t="n">
         <f aca="false">B4*C4</f>
-        <v>0.517697261552256</v>
+        <v>0.9266279936063</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="n">
+      <c r="A5" s="3" t="n">
         <v>45904</v>
       </c>
       <c r="B5" s="1" t="n">
@@ -1281,15 +1379,15 @@
       </c>
       <c r="C5" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.380751257799798</v>
+        <v>0.189830026415187</v>
       </c>
       <c r="D5" s="1" t="n">
         <f aca="false">B5*C5</f>
-        <v>0.685352264039636</v>
+        <v>0.341694047547337</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="n">
+      <c r="A6" s="3" t="n">
         <v>45905</v>
       </c>
       <c r="B6" s="1" t="n">
@@ -1297,15 +1395,15 @@
       </c>
       <c r="C6" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.156010540441412</v>
+        <v>0.814852283355914</v>
       </c>
       <c r="D6" s="1" t="n">
         <f aca="false">B6*C6</f>
-        <v>0.312021080882823</v>
+        <v>1.62970456671183</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="n">
+      <c r="A7" s="3" t="n">
         <v>45906</v>
       </c>
       <c r="B7" s="1" t="n">
@@ -1313,15 +1411,15 @@
       </c>
       <c r="C7" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.490028482048216</v>
+        <v>0.103750765726242</v>
       </c>
       <c r="D7" s="1" t="n">
         <f aca="false">B7*C7</f>
-        <v>1.07806266050608</v>
+        <v>0.228251684597733</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="n">
+      <c r="A8" s="3" t="n">
         <v>45907</v>
       </c>
       <c r="B8" s="1" t="n">
@@ -1329,15 +1427,15 @@
       </c>
       <c r="C8" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.339518823890797</v>
+        <v>0.358948618105992</v>
       </c>
       <c r="D8" s="1" t="n">
         <f aca="false">B8*C8</f>
-        <v>0.814845177337913</v>
+        <v>0.86147668345438</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="n">
+      <c r="A9" s="3" t="n">
         <v>45908</v>
       </c>
       <c r="B9" s="1" t="n">
@@ -1345,15 +1443,15 @@
       </c>
       <c r="C9" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.487747311954685</v>
+        <v>0.0319829176367099</v>
       </c>
       <c r="D9" s="1" t="n">
         <f aca="false">B9*C9</f>
-        <v>1.26814301108218</v>
+        <v>0.0831555858554458</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="n">
+      <c r="A10" s="3" t="n">
         <v>45909</v>
       </c>
       <c r="B10" s="1" t="n">
@@ -1361,15 +1459,15 @@
       </c>
       <c r="C10" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.347918120133841</v>
+        <v>0.484253456314983</v>
       </c>
       <c r="D10" s="1" t="n">
         <f aca="false">B10*C10</f>
-        <v>0.974170736374756</v>
+        <v>1.35590967768195</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="n">
+      <c r="A11" s="3" t="n">
         <v>45910</v>
       </c>
       <c r="B11" s="1" t="n">
@@ -1377,15 +1475,15 @@
       </c>
       <c r="C11" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.2255909413269</v>
+        <v>0.303775837445512</v>
       </c>
       <c r="D11" s="1" t="n">
         <f aca="false">B11*C11</f>
-        <v>0.6767728239807</v>
+        <v>0.911327512336537</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="n">
+      <c r="A12" s="3" t="n">
         <v>45911</v>
       </c>
       <c r="B12" s="1" t="n">
@@ -1393,15 +1491,15 @@
       </c>
       <c r="C12" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.660288887972121</v>
+        <v>0.381825673053932</v>
       </c>
       <c r="D12" s="1" t="n">
         <f aca="false">B12*C12</f>
-        <v>2.11292444151079</v>
+        <v>1.22184215377258</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="n">
+      <c r="A13" s="3" t="n">
         <v>45912</v>
       </c>
       <c r="B13" s="1" t="n">
@@ -1409,15 +1507,15 @@
       </c>
       <c r="C13" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.22197713055995</v>
+        <v>0.85977241884567</v>
       </c>
       <c r="D13" s="1" t="n">
         <f aca="false">B13*C13</f>
-        <v>0.754722243903829</v>
+        <v>2.92322622407528</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="n">
+      <c r="A14" s="3" t="n">
         <v>45913</v>
       </c>
       <c r="B14" s="1" t="n">
@@ -1425,15 +1523,15 @@
       </c>
       <c r="C14" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.301933192865377</v>
+        <v>0.458395906636241</v>
       </c>
       <c r="D14" s="1" t="n">
         <f aca="false">B14*C14</f>
-        <v>1.08695949431536</v>
+        <v>1.65022526389047</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="n">
+      <c r="A15" s="3" t="n">
         <v>45914</v>
       </c>
       <c r="B15" s="1" t="n">
@@ -1441,15 +1539,15 @@
       </c>
       <c r="C15" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0468912795720362</v>
+        <v>0.643837250929912</v>
       </c>
       <c r="D15" s="1" t="n">
         <f aca="false">B15*C15</f>
-        <v>0.178186862373738</v>
+        <v>2.44658155353367</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="n">
+      <c r="A16" s="3" t="n">
         <v>45915</v>
       </c>
       <c r="B16" s="1" t="n">
@@ -1457,15 +1555,15 @@
       </c>
       <c r="C16" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.623347263891054</v>
+        <v>0.541872148763174</v>
       </c>
       <c r="D16" s="1" t="n">
         <f aca="false">B16*C16</f>
-        <v>2.49338905556422</v>
+        <v>2.16748859505269</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="n">
+      <c r="A17" s="3" t="n">
         <v>45916</v>
       </c>
       <c r="B17" s="1" t="n">
@@ -1473,15 +1571,15 @@
       </c>
       <c r="C17" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0886238947883603</v>
+        <v>0.513565185708165</v>
       </c>
       <c r="D17" s="1" t="n">
         <f aca="false">B17*C17</f>
-        <v>0.372220358111113</v>
+        <v>2.15697377997429</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="n">
+      <c r="A18" s="3" t="n">
         <v>45917</v>
       </c>
       <c r="B18" s="1" t="n">
@@ -1489,15 +1587,15 @@
       </c>
       <c r="C18" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.467364827386421</v>
+        <v>0.788820738341168</v>
       </c>
       <c r="D18" s="1" t="n">
         <f aca="false">B18*C18</f>
-        <v>2.05640524050025</v>
+        <v>3.47081124870114</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="n">
+      <c r="A19" s="3" t="n">
         <v>45918</v>
       </c>
       <c r="B19" s="1" t="n">
@@ -1505,15 +1603,15 @@
       </c>
       <c r="C19" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.60263001758906</v>
+        <v>0.337952413955722</v>
       </c>
       <c r="D19" s="1" t="n">
         <f aca="false">B19*C19</f>
-        <v>2.77209808090968</v>
+        <v>1.55458110419632</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="n">
+      <c r="A20" s="3" t="n">
         <v>45919</v>
       </c>
       <c r="B20" s="1" t="n">
@@ -1521,51 +1619,51 @@
       </c>
       <c r="C20" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.479880123660462</v>
+        <v>0.515588284267414</v>
       </c>
       <c r="D20" s="1" t="n">
         <f aca="false">B20*C20</f>
-        <v>2.30342459357022</v>
+        <v>2.47482376448359</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2"/>
+      <c r="A21" s="3"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2"/>
+      <c r="A22" s="3"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2"/>
+      <c r="A23" s="3"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2"/>
+      <c r="A24" s="3"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2"/>
+      <c r="A25" s="3"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2"/>
+      <c r="A26" s="3"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="n">
+      <c r="A27" s="3" t="n">
         <v>45926</v>
       </c>
       <c r="B27" s="1" t="n">
@@ -1573,15 +1671,15 @@
       </c>
       <c r="C27" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.284438945918143</v>
+        <v>0.597101586431998</v>
       </c>
       <c r="D27" s="1" t="n">
         <f aca="false">B27*C27</f>
-        <v>1.76352146469249</v>
+        <v>3.70202983587839</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="n">
+      <c r="A28" s="3" t="n">
         <v>45927</v>
       </c>
       <c r="B28" s="1" t="n">
@@ -1589,15 +1687,15 @@
       </c>
       <c r="C28" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0652978471996168</v>
+        <v>0.517994750536849</v>
       </c>
       <c r="D28" s="1" t="n">
         <f aca="false">B28*C28</f>
-        <v>0.417906222077547</v>
+        <v>3.31516640343583</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2" t="n">
+      <c r="A29" s="3" t="n">
         <v>45928</v>
       </c>
       <c r="B29" s="1" t="n">
@@ -1605,15 +1703,15 @@
       </c>
       <c r="C29" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.614351614258322</v>
+        <v>0.973484117046345</v>
       </c>
       <c r="D29" s="1" t="n">
         <f aca="false">B29*C29</f>
-        <v>4.05472065410492</v>
+        <v>6.42499517250588</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="n">
+      <c r="A30" s="3" t="n">
         <v>45929</v>
       </c>
       <c r="B30" s="1" t="n">
@@ -1621,15 +1719,15 @@
       </c>
       <c r="C30" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.902601112006274</v>
+        <v>0.186264154111818</v>
       </c>
       <c r="D30" s="1" t="n">
         <f aca="false">B30*C30</f>
-        <v>6.13768756164267</v>
+        <v>1.26659624796036</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="n">
+      <c r="A31" s="3" t="n">
         <v>45930</v>
       </c>
       <c r="B31" s="1" t="n">
@@ -1637,11 +1735,11 @@
       </c>
       <c r="C31" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.310056468115094</v>
+        <v>0.477309277208043</v>
       </c>
       <c r="D31" s="1" t="n">
         <f aca="false">B31*C31</f>
-        <v>2.17039527680566</v>
+        <v>3.3411649404563</v>
       </c>
     </row>
   </sheetData>
@@ -1662,499 +1760,499 @@
   </sheetPr>
   <dimension ref="B2:E35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="6" t="n">
+        <v>45901</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.45182568290649</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <f aca="false">C6*D6</f>
+        <v>0.542190819487788</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="6" t="n">
+        <v>45902</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.726140479061456</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <f aca="false">C7*D7</f>
+        <v>1.01659667068604</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="6" t="n">
+        <v>45903</v>
+      </c>
+      <c r="C8" s="5" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.928428242878223</v>
+      </c>
+      <c r="E8" s="5" t="n">
+        <f aca="false">C8*D8</f>
+        <v>1.48548518860516</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="6" t="n">
+        <v>45904</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="D9" s="5" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.245145014202778</v>
+      </c>
+      <c r="E9" s="5" t="n">
+        <f aca="false">C9*D9</f>
+        <v>0.441261025565001</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="6" t="n">
+        <v>45905</v>
+      </c>
+      <c r="C10" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" s="5" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.804635439454299</v>
+      </c>
+      <c r="E10" s="5" t="n">
+        <f aca="false">C10*D10</f>
+        <v>1.6092708789086</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="6" t="n">
+        <v>45906</v>
+      </c>
+      <c r="C11" s="5" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="D11" s="5" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.334012045593343</v>
+      </c>
+      <c r="E11" s="5" t="n">
+        <f aca="false">C11*D11</f>
+        <v>0.734826500305354</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="6" t="n">
+        <v>45907</v>
+      </c>
+      <c r="C12" s="5" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="D12" s="5" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.979199812462746</v>
+      </c>
+      <c r="E12" s="5" t="n">
+        <f aca="false">C12*D12</f>
+        <v>2.35007954991059</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="6"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="6" t="n">
+        <v>45909</v>
+      </c>
+      <c r="C14" s="5" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="D14" s="5" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.403571042766327</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <f aca="false">C14*D14</f>
+        <v>1.12999891974572</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="6" t="n">
+        <v>45910</v>
+      </c>
+      <c r="C15" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D15" s="5" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.664627155463666</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <f aca="false">C15*D15</f>
+        <v>1.993881466391</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="6" t="n">
+        <v>45911</v>
+      </c>
+      <c r="C16" s="5" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="D16" s="5" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.132450951215596</v>
+      </c>
+      <c r="E16" s="5" t="n">
+        <f aca="false">C16*D16</f>
+        <v>0.423843043889909</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="6" t="n">
+        <v>45912</v>
+      </c>
+      <c r="C17" s="5" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="D17" s="5" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.76516934925232</v>
+      </c>
+      <c r="E17" s="5" t="n">
+        <f aca="false">C17*D17</f>
+        <v>2.60157578745789</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="6" t="n">
+        <v>45913</v>
+      </c>
+      <c r="C18" s="5" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="D18" s="5" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.068059086103197</v>
+      </c>
+      <c r="E18" s="5" t="n">
+        <f aca="false">C18*D18</f>
+        <v>0.245012709971509</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="6" t="n">
+        <v>45914</v>
+      </c>
+      <c r="C19" s="5" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="D19" s="5" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.897528274637036</v>
+      </c>
+      <c r="E19" s="5" t="n">
+        <f aca="false">C19*D19</f>
+        <v>3.41060744362074</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="6" t="n">
+        <v>45915</v>
+      </c>
+      <c r="C20" s="5" t="n">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="5" t="n">
-        <v>45901</v>
-      </c>
-      <c r="C6" s="4" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="D6" s="4" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.562820218499161</v>
-      </c>
-      <c r="E6" s="4" t="n">
-        <f aca="false">C6*D6</f>
-        <v>0.675384262198993</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="5" t="n">
-        <v>45902</v>
-      </c>
-      <c r="C7" s="4" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="D7" s="4" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.782557439297352</v>
-      </c>
-      <c r="E7" s="4" t="n">
-        <f aca="false">C7*D7</f>
-        <v>1.09558041501629</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="5" t="n">
-        <v>45903</v>
-      </c>
-      <c r="C8" s="4" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="D8" s="4" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.0935883001147127</v>
-      </c>
-      <c r="E8" s="4" t="n">
-        <f aca="false">C8*D8</f>
-        <v>0.14974128018354</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="5" t="n">
-        <v>45904</v>
-      </c>
-      <c r="C9" s="4" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="D9" s="4" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.364416315505873</v>
-      </c>
-      <c r="E9" s="4" t="n">
-        <f aca="false">C9*D9</f>
-        <v>0.655949367910572</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="5" t="n">
-        <v>45905</v>
-      </c>
-      <c r="C10" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D10" s="4" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.759499053723507</v>
-      </c>
-      <c r="E10" s="4" t="n">
-        <f aca="false">C10*D10</f>
-        <v>1.51899810744701</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="5" t="n">
-        <v>45906</v>
-      </c>
-      <c r="C11" s="4" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="D11" s="4" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.108946058363007</v>
-      </c>
-      <c r="E11" s="4" t="n">
-        <f aca="false">C11*D11</f>
-        <v>0.239681328398616</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="5" t="n">
-        <v>45907</v>
-      </c>
-      <c r="C12" s="4" t="n">
-        <v>2.4</v>
-      </c>
-      <c r="D12" s="4" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.379112338213373</v>
-      </c>
-      <c r="E12" s="4" t="n">
-        <f aca="false">C12*D12</f>
-        <v>0.909869611712095</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="5"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="5" t="n">
-        <v>45909</v>
-      </c>
-      <c r="C14" s="4" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="D14" s="4" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.788240508100484</v>
-      </c>
-      <c r="E14" s="4" t="n">
-        <f aca="false">C14*D14</f>
-        <v>2.20707342268136</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="5" t="n">
-        <v>45910</v>
-      </c>
-      <c r="C15" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="D15" s="4" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.388704088257291</v>
-      </c>
-      <c r="E15" s="4" t="n">
-        <f aca="false">C15*D15</f>
-        <v>1.16611226477187</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="5" t="n">
-        <v>45911</v>
-      </c>
-      <c r="C16" s="4" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="D16" s="4" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.250711678563211</v>
-      </c>
-      <c r="E16" s="4" t="n">
-        <f aca="false">C16*D16</f>
-        <v>0.802277371402275</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="5" t="n">
-        <v>45912</v>
-      </c>
-      <c r="C17" s="4" t="n">
-        <v>3.4</v>
-      </c>
-      <c r="D17" s="4" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.970293613271688</v>
-      </c>
-      <c r="E17" s="4" t="n">
-        <f aca="false">C17*D17</f>
-        <v>3.29899828512374</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="5" t="n">
-        <v>45913</v>
-      </c>
-      <c r="C18" s="4" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="D18" s="4" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.109833332851171</v>
-      </c>
-      <c r="E18" s="4" t="n">
-        <f aca="false">C18*D18</f>
-        <v>0.395399998264216</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="5" t="n">
-        <v>45914</v>
-      </c>
-      <c r="C19" s="4" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="D19" s="4" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.887470553904978</v>
-      </c>
-      <c r="E19" s="4" t="n">
-        <f aca="false">C19*D19</f>
-        <v>3.37238810483892</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="5" t="n">
-        <v>45915</v>
-      </c>
-      <c r="C20" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="D20" s="4" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.540961276882063</v>
-      </c>
-      <c r="E20" s="4" t="n">
+      <c r="D20" s="5" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.556051656130754</v>
+      </c>
+      <c r="E20" s="5" t="n">
         <f aca="false">C20*D20</f>
-        <v>2.16384510752825</v>
+        <v>2.22420662452302</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="5" t="n">
+      <c r="B21" s="6" t="n">
         <v>45916</v>
       </c>
-      <c r="C21" s="4" t="n">
+      <c r="C21" s="5" t="n">
         <v>4.2</v>
       </c>
-      <c r="D21" s="4" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.407942444953334</v>
-      </c>
-      <c r="E21" s="4" t="n">
+      <c r="D21" s="5" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.295434130653487</v>
+      </c>
+      <c r="E21" s="5" t="n">
         <f aca="false">C21*D21</f>
-        <v>1.713358268804</v>
+        <v>1.24082334874464</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="5" t="n">
+      <c r="B22" s="6" t="n">
         <v>45917</v>
       </c>
-      <c r="C22" s="4" t="n">
+      <c r="C22" s="5" t="n">
         <v>4.4</v>
       </c>
-      <c r="D22" s="4" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.0107587276576826</v>
-      </c>
-      <c r="E22" s="4" t="n">
+      <c r="D22" s="5" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.833950761860975</v>
+      </c>
+      <c r="E22" s="5" t="n">
         <f aca="false">C22*D22</f>
-        <v>0.0473384016938033</v>
+        <v>3.66938335218829</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="5" t="n">
+      <c r="B23" s="6" t="n">
         <v>45918</v>
       </c>
-      <c r="C23" s="4" t="n">
+      <c r="C23" s="5" t="n">
         <v>4.6</v>
       </c>
-      <c r="D23" s="4" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.785105241442041</v>
-      </c>
-      <c r="E23" s="4" t="n">
+      <c r="D23" s="5" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.856379034288144</v>
+      </c>
+      <c r="E23" s="5" t="n">
         <f aca="false">C23*D23</f>
-        <v>3.61148411063339</v>
+        <v>3.93934355772546</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="5" t="n">
+      <c r="B24" s="6" t="n">
         <v>45919</v>
       </c>
-      <c r="C24" s="4" t="n">
+      <c r="C24" s="5" t="n">
         <v>4.8</v>
       </c>
-      <c r="D24" s="4" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.854772440090416</v>
-      </c>
-      <c r="E24" s="4" t="n">
+      <c r="D24" s="5" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.579570592844261</v>
+      </c>
+      <c r="E24" s="5" t="n">
         <f aca="false">C24*D24</f>
-        <v>4.10290771243399</v>
+        <v>2.78193884565245</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="5" t="n">
+      <c r="B25" s="6" t="n">
         <v>45920</v>
       </c>
-      <c r="C25" s="4" t="n">
+      <c r="C25" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="D25" s="4" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.738541513372186</v>
-      </c>
-      <c r="E25" s="4" t="n">
+      <c r="D25" s="5" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.225904341915209</v>
+      </c>
+      <c r="E25" s="5" t="n">
         <f aca="false">C25*D25</f>
-        <v>3.69270756686093</v>
+        <v>1.12952170957605</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="5" t="n">
+      <c r="B26" s="6" t="n">
         <v>45921</v>
       </c>
-      <c r="C26" s="4" t="n">
+      <c r="C26" s="5" t="n">
         <v>5.2</v>
       </c>
-      <c r="D26" s="4" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.630761936458276</v>
-      </c>
-      <c r="E26" s="4" t="n">
+      <c r="D26" s="5" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.481201556212993</v>
+      </c>
+      <c r="E26" s="5" t="n">
         <f aca="false">C26*D26</f>
-        <v>3.27996206958303</v>
+        <v>2.50224809230756</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="5" t="n">
+      <c r="B27" s="6" t="n">
         <v>45922</v>
       </c>
-      <c r="C27" s="4" t="n">
+      <c r="C27" s="5" t="n">
         <v>5.4</v>
       </c>
-      <c r="D27" s="4" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.292868501995439</v>
-      </c>
-      <c r="E27" s="4" t="n">
+      <c r="D27" s="5" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.0178557148747067</v>
+      </c>
+      <c r="E27" s="5" t="n">
         <f aca="false">C27*D27</f>
-        <v>1.58148991077537</v>
+        <v>0.0964208603234159</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="5" t="n">
+      <c r="B28" s="6" t="n">
         <v>45923</v>
       </c>
-      <c r="C28" s="4" t="n">
+      <c r="C28" s="5" t="n">
         <v>5.6</v>
       </c>
-      <c r="D28" s="4" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.653816452420128</v>
-      </c>
-      <c r="E28" s="4" t="n">
+      <c r="D28" s="5" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.262939589180599</v>
+      </c>
+      <c r="E28" s="5" t="n">
         <f aca="false">C28*D28</f>
-        <v>3.66137213355272</v>
+        <v>1.47246169941136</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="5" t="n">
+      <c r="B29" s="6" t="n">
         <v>45924</v>
       </c>
-      <c r="C29" s="4" t="n">
+      <c r="C29" s="5" t="n">
         <v>5.8</v>
       </c>
-      <c r="D29" s="4" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.635161162264538</v>
-      </c>
-      <c r="E29" s="4" t="n">
+      <c r="D29" s="5" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.881285484185898</v>
+      </c>
+      <c r="E29" s="5" t="n">
         <f aca="false">C29*D29</f>
-        <v>3.68393474113432</v>
+        <v>5.11145580827821</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="5" t="n">
+      <c r="B30" s="6" t="n">
         <v>45925</v>
       </c>
-      <c r="C30" s="4" t="n">
+      <c r="C30" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="D30" s="4" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.305064555747129</v>
-      </c>
-      <c r="E30" s="4" t="n">
+      <c r="D30" s="5" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.677085456873489</v>
+      </c>
+      <c r="E30" s="5" t="n">
         <f aca="false">C30*D30</f>
-        <v>1.83038733448277</v>
+        <v>4.06251274124093</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="5" t="n">
+      <c r="B31" s="6" t="n">
         <v>45926</v>
       </c>
-      <c r="C31" s="4" t="n">
+      <c r="C31" s="5" t="n">
         <v>6.2</v>
       </c>
-      <c r="D31" s="4" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.137773030809458</v>
-      </c>
-      <c r="E31" s="4" t="n">
+      <c r="D31" s="5" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.906552071256721</v>
+      </c>
+      <c r="E31" s="5" t="n">
         <f aca="false">C31*D31</f>
-        <v>0.854192791018641</v>
+        <v>5.62062284179167</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="5" t="n">
+      <c r="B32" s="6" t="n">
         <v>45927</v>
       </c>
-      <c r="C32" s="4" t="n">
+      <c r="C32" s="5" t="n">
         <v>6.4</v>
       </c>
-      <c r="D32" s="4" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.352307823427738</v>
-      </c>
-      <c r="E32" s="4" t="n">
+      <c r="D32" s="5" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.185006099359403</v>
+      </c>
+      <c r="E32" s="5" t="n">
         <f aca="false">C32*D32</f>
-        <v>2.25477006993753</v>
+        <v>1.18403903590018</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="5" t="n">
+      <c r="B33" s="6" t="n">
         <v>45928</v>
       </c>
-      <c r="C33" s="4" t="n">
+      <c r="C33" s="5" t="n">
         <v>6.6</v>
       </c>
-      <c r="D33" s="4" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.986890237361725</v>
-      </c>
-      <c r="E33" s="4" t="n">
+      <c r="D33" s="5" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.466883922819508</v>
+      </c>
+      <c r="E33" s="5" t="n">
         <f aca="false">C33*D33</f>
-        <v>6.51347556658738</v>
+        <v>3.08143389060875</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="5" t="n">
+      <c r="B34" s="6" t="n">
         <v>45929</v>
       </c>
-      <c r="C34" s="4" t="n">
+      <c r="C34" s="5" t="n">
         <v>6.8</v>
       </c>
-      <c r="D34" s="4" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.037213003376413</v>
-      </c>
-      <c r="E34" s="4" t="n">
+      <c r="D34" s="5" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.125568078991259</v>
+      </c>
+      <c r="E34" s="5" t="n">
         <f aca="false">C34*D34</f>
-        <v>0.253048422959608</v>
+        <v>0.853862937140561</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="5" t="n">
+      <c r="B35" s="6" t="n">
         <v>45930</v>
       </c>
-      <c r="C35" s="4" t="n">
+      <c r="C35" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="D35" s="4" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.692428149632797</v>
-      </c>
-      <c r="E35" s="4" t="n">
+      <c r="D35" s="5" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.749975910149886</v>
+      </c>
+      <c r="E35" s="5" t="n">
         <f aca="false">C35*D35</f>
-        <v>4.84699704742958</v>
+        <v>5.24983137104921</v>
       </c>
     </row>
   </sheetData>

</xml_diff>